<commit_message>
reorganized notbook file location
</commit_message>
<xml_diff>
--- a/raw_data/IVM6311_Testing_scripts.xlsx
+++ b/raw_data/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harkum\Documents\6311\Software\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F67A20A-DCF4-4F60-8310-7CCBB285A1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3733C-D6AA-4CF4-AA60-44DF3DEB71AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -18140,6 +18140,24 @@
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -18164,24 +18182,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18578,8 +18578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D91B9C-5E8C-479A-83F9-A38D53329BF0}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18590,10 +18590,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="117"/>
       <c r="C1" s="17" t="s">
         <v>5</v>
       </c>
@@ -18618,10 +18618,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
@@ -18633,10 +18633,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
@@ -18648,8 +18648,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="273" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
-      <c r="B5" s="109"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="37" t="s">
         <v>13</v>
       </c>
@@ -18661,7 +18661,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="120" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -18678,7 +18678,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A7" s="110"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
@@ -18693,7 +18693,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A8" s="110"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
@@ -18708,7 +18708,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A9" s="110"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
@@ -18723,7 +18723,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A10" s="110"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
@@ -19375,7 +19375,7 @@
   <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19388,10 +19388,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="117"/>
       <c r="C1" s="17" t="s">
         <v>5</v>
       </c>
@@ -19438,10 +19438,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="15" t="s">
         <v>64</v>
       </c>
@@ -19465,10 +19465,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="9" t="s">
         <v>69</v>
       </c>
@@ -19492,8 +19492,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
-      <c r="B5" s="109"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="37" t="s">
         <v>312</v>
       </c>
@@ -19517,7 +19517,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="120" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -19538,7 +19538,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="110"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
@@ -19553,7 +19553,7 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="110"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
@@ -19580,7 +19580,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="110"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
@@ -19599,7 +19599,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="110"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
@@ -20850,10 +20850,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="111"/>
+      <c r="B1" s="121"/>
       <c r="C1" s="17" t="s">
         <v>95</v>
       </c>
@@ -21014,10 +21014,10 @@
       </c>
     </row>
     <row r="3" spans="1:28" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="111"/>
+      <c r="B3" s="121"/>
       <c r="C3" s="64" t="s">
         <v>64</v>
       </c>
@@ -21098,10 +21098,10 @@
       </c>
     </row>
     <row r="4" spans="1:28" s="1" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="111"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="65" t="s">
         <v>115</v>
       </c>
@@ -21182,8 +21182,8 @@
       </c>
     </row>
     <row r="5" spans="1:28" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="102" t="s">
         <v>141</v>
       </c>
@@ -21264,7 +21264,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="124" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -21342,7 +21342,7 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="114"/>
+      <c r="A7" s="124"/>
       <c r="B7" s="60" t="s">
         <v>17</v>
       </c>
@@ -21374,7 +21374,7 @@
       <c r="AB7" s="68"/>
     </row>
     <row r="8" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="114"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="61" t="s">
         <v>19</v>
       </c>
@@ -21424,7 +21424,7 @@
       <c r="AB8" s="69"/>
     </row>
     <row r="9" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="114"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="62" t="s">
         <v>21</v>
       </c>
@@ -21500,7 +21500,7 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="114"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="60" t="s">
         <v>22</v>
       </c>
@@ -24906,8 +24906,8 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24927,10 +24927,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="111"/>
+      <c r="B1" s="121"/>
       <c r="C1" s="17" t="s">
         <v>5</v>
       </c>
@@ -25025,10 +25025,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="111"/>
+      <c r="B3" s="121"/>
       <c r="C3" s="15" t="s">
         <v>68</v>
       </c>
@@ -25076,10 +25076,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="111"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="65" t="s">
         <v>183</v>
       </c>
@@ -25127,8 +25127,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="104" t="s">
         <v>198</v>
       </c>
@@ -25176,7 +25176,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="124" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -25199,7 +25199,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="114"/>
+      <c r="A7" s="124"/>
       <c r="B7" s="60" t="s">
         <v>17</v>
       </c>
@@ -25220,7 +25220,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="114"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="61" t="s">
         <v>19</v>
       </c>
@@ -25265,7 +25265,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="114"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="62" t="s">
         <v>21</v>
       </c>
@@ -25290,7 +25290,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="114"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="60" t="s">
         <v>22</v>
       </c>
@@ -27441,7 +27441,7 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -27455,10 +27455,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="117"/>
       <c r="C1" s="17" t="s">
         <v>95</v>
       </c>
@@ -27525,10 +27525,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="15" t="s">
         <v>65</v>
       </c>
@@ -27562,10 +27562,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="9" t="s">
         <v>321</v>
       </c>
@@ -27591,12 +27591,12 @@
       <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
-      <c r="B5" s="108"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="56" t="s">
         <v>327</v>
       </c>
-      <c r="D5" s="115" t="str">
+      <c r="D5" s="107" t="str">
         <f>TRIM(SUBSTITUTE(C5,CHAR(32),""))</f>
         <v xml:space="preserve">DAC-PAANALOG_IN_DC_COUPLED
 ForceANA__-6_00x03_0x04"EnabledigitaltestFSYN"0x04_0x112"Enabledigitaltestana_azcomp_out"0x17_0x01"force_dig_azcomp_en"0x17_0x00"force_dig_azcomp_az"0xFE_0x00"Returnpage0"Measure__Voltage__FSYN
@@ -27631,7 +27631,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="120" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -27650,7 +27650,7 @@
       <c r="M6" s="38"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="110"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
@@ -27667,7 +27667,7 @@
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="110"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
@@ -27704,12 +27704,12 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="110"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
@@ -27721,7 +27721,7 @@
       <c r="M9" s="39"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="110"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
@@ -27956,14 +27956,14 @@
       <c r="B17" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="109" t="s">
         <v>341</v>
       </c>
-      <c r="D17" s="117"/>
+      <c r="D17" s="109"/>
       <c r="E17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="118" t="s">
+      <c r="F17" s="110" t="s">
         <v>93</v>
       </c>
       <c r="G17" s="50" t="s">
@@ -28222,8 +28222,8 @@
     <row r="29" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="43"/>
       <c r="B29" s="40"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="111"/>
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
@@ -28237,8 +28237,8 @@
     <row r="30" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="52"/>
       <c r="B30" s="40"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
@@ -28252,8 +28252,8 @@
     <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="53"/>
       <c r="B31" s="42"/>
-      <c r="C31" s="121"/>
-      <c r="D31" s="122"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="114"/>
       <c r="E31" s="51"/>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -28267,8 +28267,8 @@
     <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47"/>
       <c r="B32" s="55"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="122"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="114"/>
       <c r="E32" s="51"/>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -28282,8 +28282,8 @@
     <row r="33" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="123"/>
-      <c r="D33" s="122"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="114"/>
       <c r="E33" s="51"/>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -28297,8 +28297,8 @@
     <row r="34" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="47"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="123"/>
-      <c r="D34" s="122"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="114"/>
       <c r="E34" s="51"/>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -28312,8 +28312,8 @@
     <row r="35" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="47"/>
       <c r="B35" s="40"/>
-      <c r="C35" s="123"/>
-      <c r="D35" s="122"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="114"/>
       <c r="E35" s="51"/>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -28327,8 +28327,8 @@
     <row r="36" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="47"/>
       <c r="B36" s="40"/>
-      <c r="C36" s="123"/>
-      <c r="D36" s="122"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="51"/>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -28342,8 +28342,8 @@
     <row r="37" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47"/>
       <c r="B37" s="40"/>
-      <c r="C37" s="123"/>
-      <c r="D37" s="122"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="51"/>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -28357,8 +28357,8 @@
     <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="47"/>
       <c r="B38" s="42"/>
-      <c r="C38" s="123"/>
-      <c r="D38" s="122"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="51"/>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -28372,8 +28372,8 @@
     <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="47"/>
       <c r="B39" s="42"/>
-      <c r="C39" s="123"/>
-      <c r="D39" s="122"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="114"/>
       <c r="E39" s="51"/>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -28387,8 +28387,8 @@
     <row r="40" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="47"/>
       <c r="B40" s="40"/>
-      <c r="C40" s="123"/>
-      <c r="D40" s="122"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="114"/>
       <c r="E40" s="51"/>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -28402,8 +28402,8 @@
     <row r="41" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="47"/>
       <c r="B41" s="40"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="122"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="114"/>
       <c r="E41" s="51"/>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
@@ -28417,8 +28417,8 @@
     <row r="42" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47"/>
       <c r="B42" s="40"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="122"/>
+      <c r="C42" s="115"/>
+      <c r="D42" s="114"/>
       <c r="E42" s="51"/>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
@@ -28432,8 +28432,8 @@
     <row r="43" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="47"/>
       <c r="B43" s="40"/>
-      <c r="C43" s="123"/>
-      <c r="D43" s="122"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="114"/>
       <c r="E43" s="51"/>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
@@ -28447,8 +28447,8 @@
     <row r="44" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="47"/>
       <c r="B44" s="40"/>
-      <c r="C44" s="123"/>
-      <c r="D44" s="122"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="114"/>
       <c r="E44" s="51"/>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -28462,8 +28462,8 @@
     <row r="45" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="47"/>
       <c r="B45" s="41"/>
-      <c r="C45" s="123"/>
-      <c r="D45" s="122"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="114"/>
       <c r="E45" s="51"/>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -28477,8 +28477,8 @@
     <row r="46" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="47"/>
       <c r="B46" s="41"/>
-      <c r="C46" s="123"/>
-      <c r="D46" s="122"/>
+      <c r="C46" s="115"/>
+      <c r="D46" s="114"/>
       <c r="E46" s="51"/>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
@@ -28492,8 +28492,8 @@
     <row r="47" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="47"/>
       <c r="B47" s="41"/>
-      <c r="C47" s="123"/>
-      <c r="D47" s="122"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="114"/>
       <c r="E47" s="51"/>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -28507,8 +28507,8 @@
     <row r="48" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="47"/>
       <c r="B48" s="41"/>
-      <c r="C48" s="123"/>
-      <c r="D48" s="122"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="114"/>
       <c r="E48" s="51"/>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -28522,8 +28522,8 @@
     <row r="49" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="47"/>
       <c r="B49" s="41"/>
-      <c r="C49" s="123"/>
-      <c r="D49" s="122"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="114"/>
       <c r="E49" s="51"/>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -28537,8 +28537,8 @@
     <row r="50" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A50" s="47"/>
       <c r="B50" s="41"/>
-      <c r="C50" s="123"/>
-      <c r="D50" s="122"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="114"/>
       <c r="E50" s="51"/>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -28552,8 +28552,8 @@
     <row r="51" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="48"/>
       <c r="B51" s="44"/>
-      <c r="C51" s="124"/>
-      <c r="D51" s="124"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
       <c r="E51" s="50"/>
       <c r="F51" s="50"/>
       <c r="G51" s="50"/>
@@ -29683,6 +29683,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -29899,17 +29910,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29920,6 +29920,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29938,23 +29955,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
save instruction extraction and testing added
</commit_message>
<xml_diff>
--- a/raw_data/IVM6311_Testing_scripts.xlsx
+++ b/raw_data/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harkum\Documents\6311\Software\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8669AE72-9270-425A-A939-AE08AC1FE37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801D9AD1-FADA-4F8F-9AF5-3BD818041DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61332" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -8002,374 +8002,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_Startup
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"in base page"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x11[1:0]_2b00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Input mode: TDM"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x32_0x41</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "setting FSYN rate=384kHz and OSR=20"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE0[1:0]_2b00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Calibration time 600us, change in case of issues"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE0[3:2]_2b00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "AZ mode time 300us, change in case of issues"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE2[0]_1b1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Internal calibration start"
-Wait__delay__20ms
-Read__E5 "bit[4] =1 indicates end of calibration"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"in test page"
-Read__CA-CC "OTP cal registers CA-CC in page 1 are written, not possible to measure analog value"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in base page"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xE2_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Reset internal calibration bit"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE2[0]_0x02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "External calibration start"
-Wait__delay__20ms
-Read__E5 "bit[4] =1 indicates end of calibration"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"in test page"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Read__CD-CF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OTP cal registers CD-CF in page 1 are written, (difference btw ext-int values), it is possible to measure analog value"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in base page"
-0x50[0]_1b0 "noise gate disabling"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DACPA_tourn _on_wo_calibration
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__10ms
-Read__17 "check result 0x0A to be in playback mode"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__EXT_IDLE_OFFSET__diff__OUTP__OUTM
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" we've measured the offset when the part will be in idle mode"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in test page"
-Save_CB_varCB "int offset idle"
-Save_CC_varCC "int offset idle"
-Save_CE_varCE "diff. ext-int in idle"
-Save_CF_varCF "diff. ext-int in idle"
-Copy__0xCB[7:4]__0xCC[3:0] "int/ext zero copied in int/ext idle"
-Copy__0xCA[7:4]__0xCB[3:0] "int/ext zero copied in int/ext idle"
-Copy__0xCA[3:0]__0xCC[7:4] "int/ext zero copied in int/ext idle"
-"This work-around has to be done because there is not the possibility to block idle offset ramp when we wont to measure zero register offset"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__EXT_ZERO_OFFSET__diff__OUTP__OUTM
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" we've measured the offset when the part will has zero signal"
-Restore_varCB_CB "int offset idle"
-Restore_varCC_CC "int offset idle"
-Restore_varCE_CE "diff. ext-int in idle"
-Restore_varCF_CF "diff. ext-int in idle"
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">DAC-PA TDM_768_IN
 ForceTDM__-6_1000
 Measure__THD__AP
@@ -17099,6 +16731,374 @@
   </si>
   <si>
     <t>Measure Current/Mid/Low</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_Startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"in base page"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x11[1:0]_2b00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Input mode: TDM"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x32_0x41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "setting FSYN rate=384kHz and OSR=20"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE0[1:0]_2b00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Calibration time 600us, change in case of issues"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE0[3:2]_2b00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "AZ mode time 300us, change in case of issues"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE2[0]_1b1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Internal calibration start"
+Wait__delay__20ms
+Read__E5 "bit[4] =1 indicates end of calibration"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"in test page"
+Read__CA-CC "OTP cal registers CA-CC in page 1 are written, not possible to measure analog value"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in base page"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xE2_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Reset internal calibration bit"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE2[0]_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "External calibration start"
+Wait__delay__20ms
+Read__E5 "bit[4] =1 indicates end of calibration"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"in test page"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Read__CD-CF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OTP cal registers CD-CF in page 1 are written, (difference btw ext-int values), it is possible to measure analog value"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in base page"
+0x50[0]_1b0 "noise gate disabling"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DACPA_tourn _on_wo_calibration
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__10ms
+Read__17 "check result 0x0A to be in playback mode"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__EXT_IDLE_OFFSET__diff__OUTP__OUTM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" we've measured the offset when the part will be in idle mode"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in test page"
+Save__0xCB__varCB "int offset idle"
+Save__0xCC__varCC "int offset idle"
+Save__0xCE__varCE "diff. ext-int in idle"
+Save__0xCF__varCF "diff. ext-int in idle"
+Copy__0xCB[7:4]__0xCC[3:0] "int/ext zero copied in int/ext idle"
+Copy__0xCA[7:4]__0xCB[3:0] "int/ext zero copied in int/ext idle"
+Copy__0xCA[3:0]__0xCC[7:4] "int/ext zero copied in int/ext idle"
+"This work-around has to be done because there is not the possibility to block idle offset ramp when we wont to measure zero register offset"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__EXT_ZERO_OFFSET__diff__OUTP__OUTM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" we've measured the offset when the part will has zero signal"
+Restore_varCB_CB "int offset idle"
+Restore_varCC_CC "int offset idle"
+Restore_varCE_CE "diff. ext-int in idle"
+Restore_varCF_CF "diff. ext-int in idle"
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -18654,7 +18654,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E5" s="56" t="s">
         <v>14</v>
@@ -19495,7 +19495,7 @@
       <c r="A5" s="118"/>
       <c r="B5" s="119"/>
       <c r="C5" s="37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>76</v>
@@ -21191,25 +21191,25 @@
         <v>142</v>
       </c>
       <c r="E5" s="102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F5" s="102" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G5" s="102" t="s">
         <v>143</v>
       </c>
       <c r="H5" s="95" t="s">
+        <v>306</v>
+      </c>
+      <c r="I5" s="95" t="s">
         <v>307</v>
       </c>
-      <c r="I5" s="95" t="s">
-        <v>308</v>
-      </c>
       <c r="J5" s="95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K5" s="95" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L5" s="102" t="s">
         <v>144</v>
@@ -21233,7 +21233,7 @@
         <v>150</v>
       </c>
       <c r="S5" s="95" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T5" s="95" t="s">
         <v>151</v>
@@ -21245,7 +21245,7 @@
         <v>153</v>
       </c>
       <c r="W5" s="96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="X5" s="97" t="s">
         <v>154</v>
@@ -21254,13 +21254,13 @@
         <v>155</v>
       </c>
       <c r="Z5" s="97" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AA5" s="106" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB5" s="106" t="s">
         <v>315</v>
-      </c>
-      <c r="AB5" s="106" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -25132,47 +25132,47 @@
       <c r="C5" s="104" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="E5" s="88" t="s">
         <v>199</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="F5" s="88" t="s">
         <v>200</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="G5" s="88" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="88" t="s">
+      <c r="H5" s="88" t="s">
         <v>202</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="I5" s="88" t="s">
         <v>203</v>
       </c>
-      <c r="I5" s="88" t="s">
+      <c r="J5" s="88" t="s">
         <v>204</v>
       </c>
-      <c r="J5" s="88" t="s">
+      <c r="K5" s="88" t="s">
         <v>205</v>
       </c>
-      <c r="K5" s="88" t="s">
+      <c r="L5" s="88" t="s">
         <v>206</v>
       </c>
-      <c r="L5" s="88" t="s">
+      <c r="M5" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="M5" s="56" t="s">
+      <c r="N5" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="O5" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="P5" s="56" t="s">
         <v>210</v>
       </c>
-      <c r="P5" s="56" t="s">
+      <c r="Q5" s="56" t="s">
         <v>211</v>
-      </c>
-      <c r="Q5" s="56" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -25227,41 +25227,41 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="P8" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="O8" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -25273,7 +25273,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -25316,47 +25316,47 @@
         <v>24</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>222</v>
-      </c>
       <c r="O11" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -25676,13 +25676,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="E20" s="50" t="s">
-        <v>225</v>
-      </c>
       <c r="F20" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G20" s="90"/>
       <c r="I20" s="76"/>
@@ -25703,29 +25703,29 @@
         <v>48</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="E21" s="50" t="s">
         <v>227</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>228</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="H21" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="I21" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="I21" s="76" t="s">
-        <v>231</v>
-      </c>
       <c r="J21" s="76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -25742,31 +25742,31 @@
         <v>50</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="F22" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="F22" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="G22" s="50" t="s">
+      <c r="H22" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="I22" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="J22" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="J22" s="76" t="s">
+      <c r="K22" s="76" t="s">
         <v>237</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>238</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -25852,31 +25852,31 @@
         <v>58</v>
       </c>
       <c r="C26" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="F26" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="E26" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>240</v>
-      </c>
       <c r="G26" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -25893,31 +25893,31 @@
         <v>60</v>
       </c>
       <c r="C27" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="E27" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="F27" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>240</v>
-      </c>
       <c r="G27" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -27567,23 +27567,23 @@
       </c>
       <c r="B4" s="117"/>
       <c r="C4" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>325</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -27594,7 +27594,7 @@
       <c r="A5" s="118"/>
       <c r="B5" s="118"/>
       <c r="C5" s="56" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D5" s="107" t="str">
         <f>TRIM(SUBSTITUTE(C5,CHAR(32),""))</f>
@@ -27603,31 +27603,31 @@
 </v>
       </c>
       <c r="E5" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>328</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="G5" s="56" t="s">
         <v>329</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="H5" s="56" t="s">
         <v>330</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="I5" s="56" t="s">
         <v>331</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="J5" s="56" t="s">
         <v>332</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="K5" s="56" t="s">
         <v>333</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="L5" s="56" t="s">
         <v>334</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="M5" s="56" t="s">
         <v>335</v>
-      </c>
-      <c r="M5" s="56" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -27676,31 +27676,31 @@
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>338</v>
-      </c>
       <c r="G8" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -27957,7 +27957,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="109" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D17" s="109"/>
       <c r="E17" s="50" t="s">
@@ -29398,84 +29398,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="C1" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="D1" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="E1" s="57" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>246</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>252</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="92" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="103" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>311</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="E2" s="105" t="s">
         <v>256</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="F2" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="G2" s="105" t="s">
         <v>258</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="H2" s="105" t="s">
         <v>259</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="I2" s="105" t="s">
         <v>260</v>
       </c>
-      <c r="I2" s="105" t="s">
+      <c r="J2" s="105" t="s">
         <v>261</v>
       </c>
-      <c r="J2" s="105" t="s">
+      <c r="K2" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="L2" s="105" t="s">
         <v>263</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="M2" s="105" t="s">
         <v>264</v>
-      </c>
-      <c r="M2" s="105" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -29488,7 +29488,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29504,177 +29504,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>266</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>268</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>279</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" s="89"/>
       <c r="C8" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>285</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>286</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>287</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>289</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>291</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>293</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>295</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>297</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>299</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>301</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>303</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>305</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -29683,6 +29683,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -29899,17 +29910,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29920,6 +29920,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29938,23 +29955,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
restore instruction parsed and tested
</commit_message>
<xml_diff>
--- a/raw_data/IVM6311_Testing_scripts.xlsx
+++ b/raw_data/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harkum\Documents\6311\Software\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801D9AD1-FADA-4F8F-9AF5-3BD818041DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE12B7-4E3C-43D5-9E00-E6021F92587E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17093,10 +17093,10 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">" we've measured the offset when the part will has zero signal"
-Restore_varCB_CB "int offset idle"
-Restore_varCC_CC "int offset idle"
-Restore_varCE_CE "diff. ext-int in idle"
-Restore_varCF_CF "diff. ext-int in idle"
+Restore__varCB__0xCB "int offset idle"
+Restore__varCC__0x+D5CC "int offset idle"
+Restore__varCE__0xCE "diff. ext-int in idle"
+Restore__varCF__0xCF "diff. ext-int in idle"
 </t>
     </r>
   </si>
@@ -24906,7 +24906,7 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -29683,17 +29683,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -29910,6 +29899,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29920,23 +29920,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29955,6 +29938,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>

</xml_diff>